<commit_message>
pushing changes to Timeline and Rh
</commit_message>
<xml_diff>
--- a/publication/web-root/matchsync/0.1.1/CodeSystem-glstring-codesystem.xlsx
+++ b/publication/web-root/matchsync/0.1.1/CodeSystem-glstring-codesystem.xlsx
@@ -29,7 +29,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.1</t>
+    <t>0.1.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -59,7 +59,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-02T18:26:03-06:00</t>
+    <t>2025-04-15T15:35:56-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>